<commit_message>
feature: Implement Create New button functionality, including error handling
</commit_message>
<xml_diff>
--- a/feature_list.xlsx
+++ b/feature_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56a0b29041615ddb/TreeHouse/Full-Stack Javascript/001_Vue_Basics/THFSTUTP03_Skimmit_News/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\TreeHouse\Full-Stack Javascript\001_Vue_Basics\THFSTUTP03_Skimmit_News\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5ADF106-C147-47DC-8400-927E5C1C927D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{B5ADF106-C147-47DC-8400-927E5C1C927D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{76512625-ED77-4E34-8AA1-5D88353BD668}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="1560" windowWidth="29040" windowHeight="11970" xr2:uid="{7B1C8B90-67B2-4579-A646-F32098C3620C}"/>
+    <workbookView xWindow="28800" yWindow="780" windowWidth="29040" windowHeight="11970" xr2:uid="{7B1C8B90-67B2-4579-A646-F32098C3620C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>OK</t>
   </si>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2308F4B-46A4-4C28-9CAC-946748F60FDA}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,6 +473,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feature: Implement sorting by vote count to posts list rendering
</commit_message>
<xml_diff>
--- a/feature_list.xlsx
+++ b/feature_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\TreeHouse\Full-Stack Javascript\001_Vue_Basics\THFSTUTP03_Skimmit_News\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{B5ADF106-C147-47DC-8400-927E5C1C927D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{76512625-ED77-4E34-8AA1-5D88353BD668}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{B5ADF106-C147-47DC-8400-927E5C1C927D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{017707BC-ED7C-4CE2-B889-A7B915293ECD}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="780" windowWidth="29040" windowHeight="11970" xr2:uid="{7B1C8B90-67B2-4579-A646-F32098C3620C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="3">
   <si>
     <t>OK</t>
   </si>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2308F4B-46A4-4C28-9CAC-946748F60FDA}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,6 +493,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>